<commit_message>
Datos de 11 colonias
</commit_message>
<xml_diff>
--- a/Datos_colonia.xlsx
+++ b/Datos_colonia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\IA\ia_dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roxy_\Documents\MCC\2022-1\Inteligencia Artificial\Proyecto\ia_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE45DC4-D898-4C6A-81D5-6C8E250E65D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A43171-2766-4761-AD75-BCE34DE21669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>remplaza tus datos aqui</t>
+    <t>Miramar</t>
+  </si>
+  <si>
+    <t>Lomas de Zapopan</t>
+  </si>
+  <si>
+    <t>Tabachines</t>
+  </si>
+  <si>
+    <t>Jardines Alcalde</t>
+  </si>
+  <si>
+    <t>San Juan de Dios</t>
+  </si>
+  <si>
+    <t>La Calma</t>
+  </si>
+  <si>
+    <t>Ladrón de Guevara</t>
+  </si>
+  <si>
+    <t>Ciudad Granja</t>
+  </si>
+  <si>
+    <t>Analco</t>
+  </si>
+  <si>
+    <t>Mirador San Isidro</t>
+  </si>
+  <si>
+    <t>Ciudad del Sol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +100,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -345,20 +390,789 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="17" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B1" s="1">
+        <v>44075</v>
+      </c>
+      <c r="C1" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D1" s="1">
+        <v>44136</v>
+      </c>
+      <c r="E1" s="1">
+        <v>44166</v>
+      </c>
+      <c r="F1" s="1">
+        <v>44197</v>
+      </c>
+      <c r="G1" s="1">
+        <v>44228</v>
+      </c>
+      <c r="H1" s="1">
+        <v>44256</v>
+      </c>
+      <c r="I1" s="1">
+        <v>44287</v>
+      </c>
+      <c r="J1" s="1">
+        <v>44317</v>
+      </c>
+      <c r="K1" s="1">
+        <v>44348</v>
+      </c>
+      <c r="L1" s="1">
+        <v>44378</v>
+      </c>
+      <c r="M1" s="1">
+        <v>44409</v>
+      </c>
+      <c r="N1" s="1">
+        <v>44440</v>
+      </c>
+      <c r="O1" s="1">
+        <v>44470</v>
+      </c>
+      <c r="P1" s="1">
+        <v>44501</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>44531</v>
+      </c>
+      <c r="R1" s="1">
+        <v>44562</v>
+      </c>
+      <c r="S1" s="1">
+        <v>44593</v>
+      </c>
+      <c r="T1" s="1">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="2">
+        <v>1450000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1620000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1660000</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1660000</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1650000</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1670000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1670000</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1720000</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1720000</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1720000</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1720000</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1770000</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1770000</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1770000</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1820000</v>
+      </c>
+      <c r="T2" s="2">
+        <v>1820000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1860000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1860000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1870000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2020000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1770000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1770000</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1770000</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1860000</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1860000</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1870000</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1910000</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1870000</v>
+      </c>
+      <c r="N3" s="2">
+        <v>2130000</v>
+      </c>
+      <c r="O3" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="P3" s="2">
+        <v>2190000</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2380000</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2460000</v>
+      </c>
+      <c r="S3" s="2">
+        <v>2580000</v>
+      </c>
+      <c r="T3" s="2">
+        <v>2610000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2660000</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2650000</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2650000</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2610000</v>
+      </c>
+      <c r="O4" s="2">
+        <v>2580000</v>
+      </c>
+      <c r="P4" s="2">
+        <v>2560000</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>2350000</v>
+      </c>
+      <c r="R4" s="2">
+        <v>2260000</v>
+      </c>
+      <c r="S4" s="2">
+        <v>2260000</v>
+      </c>
+      <c r="T4" s="2">
+        <v>2260000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2940000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2950000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2970000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3140000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3210000</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3250000</v>
+      </c>
+      <c r="K5" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3150000</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3100000</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="O5" s="2">
+        <v>3070000</v>
+      </c>
+      <c r="P5" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>2940000</v>
+      </c>
+      <c r="R5" s="2">
+        <v>2900000</v>
+      </c>
+      <c r="S5" s="2">
+        <v>2900000</v>
+      </c>
+      <c r="T5" s="2">
+        <v>2870000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1960000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1880000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1960000</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1960000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1960000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2150000</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2350000</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2350000</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2350000</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2350000</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2350000</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="S6" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="T6" s="2">
+        <v>2040000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4230000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4230000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4230000</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4270000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4320000</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4320000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4320000</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4320000</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4320000</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4270000</v>
+      </c>
+      <c r="L7" s="2">
+        <v>4090000</v>
+      </c>
+      <c r="M7" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="P7" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="R7" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="S7" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="T7" s="2">
+        <v>3930000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2940000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2950000</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2970000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3140000</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3210000</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3250000</v>
+      </c>
+      <c r="K8" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="L8" s="2">
+        <v>3150000</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3100000</v>
+      </c>
+      <c r="N8" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="O8" s="2">
+        <v>3070000</v>
+      </c>
+      <c r="P8" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>2940000</v>
+      </c>
+      <c r="R8" s="2">
+        <v>2900000</v>
+      </c>
+      <c r="S8" s="2">
+        <v>2900000</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2870000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3890000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3890000</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3910000</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3910000</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3980000</v>
+      </c>
+      <c r="K9" s="2">
+        <v>4110000</v>
+      </c>
+      <c r="L9" s="2">
+        <v>4080000</v>
+      </c>
+      <c r="M9" s="2">
+        <v>4080000</v>
+      </c>
+      <c r="N9" s="2">
+        <v>4130000</v>
+      </c>
+      <c r="O9" s="2">
+        <v>4110000</v>
+      </c>
+      <c r="P9" s="2">
+        <v>4180000</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>4180000</v>
+      </c>
+      <c r="R9" s="2">
+        <v>4130000</v>
+      </c>
+      <c r="S9" s="2">
+        <v>4160000</v>
+      </c>
+      <c r="T9" s="2">
+        <v>4160000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1630000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1650000</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1650000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1670000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1670000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1700000</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1780000</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1870000</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1870000</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1850000</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1940000</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1940000</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2010000</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2030000</v>
+      </c>
+      <c r="P10" s="2">
+        <v>2030000</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>2030000</v>
+      </c>
+      <c r="R10" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="S10" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="T10" s="2">
+        <v>2040000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>280000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>280000</v>
+      </c>
+      <c r="I11" s="2">
+        <v>280000</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="L11" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="M11" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="N11" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2770000</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2770000</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>280000</v>
+      </c>
+      <c r="R11" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="S11" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="T11" s="2">
+        <v>2990000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4030000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4030000</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4030000</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4110000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4180000</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4230000</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4380000</v>
+      </c>
+      <c r="I12" s="2">
+        <v>4430000</v>
+      </c>
+      <c r="J12" s="2">
+        <v>4500000</v>
+      </c>
+      <c r="K12" s="2">
+        <v>4480000</v>
+      </c>
+      <c r="L12" s="2">
+        <v>4470000</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4520000</v>
+      </c>
+      <c r="N12" s="2">
+        <v>4530000</v>
+      </c>
+      <c r="O12" s="2">
+        <v>4550000</v>
+      </c>
+      <c r="P12" s="2">
+        <v>4600000</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>4530000</v>
+      </c>
+      <c r="R12" s="2">
+        <v>4590000</v>
+      </c>
+      <c r="S12" s="2">
+        <v>4620000</v>
+      </c>
+      <c r="T12" s="2">
+        <v>4670000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Base de datos actualizado
</commit_message>
<xml_diff>
--- a/Datos_colonia.xlsx
+++ b/Datos_colonia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\IA\ia_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE45DC4-D898-4C6A-81D5-6C8E250E65D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4045510A-9869-44AC-99D8-25B3EF352803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>remplaza tus datos aqui</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Loma bonita sur</t>
+  </si>
+  <si>
+    <t>Solares</t>
+  </si>
+  <si>
+    <t>Valle imperial</t>
+  </si>
+  <si>
+    <t>Puerta de Hierro</t>
+  </si>
+  <si>
+    <t>Americana</t>
+  </si>
+  <si>
+    <t>Atlas</t>
+  </si>
+  <si>
+    <t>C.U.</t>
+  </si>
+  <si>
+    <t>Los Colomos</t>
+  </si>
+  <si>
+    <t>Chapalita</t>
+  </si>
+  <si>
+    <t>Guadalajara Centro</t>
+  </si>
+  <si>
+    <t>Bosques de la victoria</t>
+  </si>
+  <si>
+    <t>providencia 1a secc</t>
+  </si>
+  <si>
+    <t>Ladrón de Guevara</t>
+  </si>
+  <si>
+    <t>Ciudad Granja</t>
+  </si>
+  <si>
+    <t>Analco</t>
+  </si>
+  <si>
+    <t>Mirador San Isidro</t>
+  </si>
+  <si>
+    <t>Ciudad del Sol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +118,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -345,17 +407,1128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
+        <v>44075</v>
+      </c>
+      <c r="C1" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D1" s="1">
+        <v>44136</v>
+      </c>
+      <c r="E1" s="1">
+        <v>44166</v>
+      </c>
+      <c r="F1" s="1">
+        <v>44197</v>
+      </c>
+      <c r="G1" s="1">
+        <v>44228</v>
+      </c>
+      <c r="H1" s="1">
+        <v>44256</v>
+      </c>
+      <c r="I1" s="1">
+        <v>44287</v>
+      </c>
+      <c r="J1" s="1">
+        <v>44317</v>
+      </c>
+      <c r="K1" s="1">
+        <v>44348</v>
+      </c>
+      <c r="L1" s="1">
+        <v>44378</v>
+      </c>
+      <c r="M1" s="1">
+        <v>44409</v>
+      </c>
+      <c r="N1" s="1">
+        <v>44440</v>
+      </c>
+      <c r="O1" s="1">
+        <v>44470</v>
+      </c>
+      <c r="P1" s="1">
+        <v>44501</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>44531</v>
+      </c>
+      <c r="R1" s="1">
+        <v>44562</v>
+      </c>
+      <c r="S1" s="1">
+        <v>44593</v>
+      </c>
+      <c r="T1" s="1">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4120000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4130000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4130000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4120000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4250000</v>
+      </c>
+      <c r="G2" s="2">
+        <v>4250000</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4380000</v>
+      </c>
+      <c r="I2" s="2">
+        <v>4430000</v>
+      </c>
+      <c r="J2" s="2">
+        <v>5020000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>5020000</v>
+      </c>
+      <c r="L2" s="2">
+        <v>5020000</v>
+      </c>
+      <c r="M2" s="2">
+        <v>4700000</v>
+      </c>
+      <c r="N2" s="2">
+        <v>4700000</v>
+      </c>
+      <c r="O2" s="2">
+        <v>4700000</v>
+      </c>
+      <c r="P2" s="2">
+        <v>4700000</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>4700000</v>
+      </c>
+      <c r="R2" s="2">
+        <v>5020000</v>
+      </c>
+      <c r="S2" s="2">
+        <v>5020000</v>
+      </c>
+      <c r="T2" s="2">
+        <v>5020000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5120000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5120000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5160000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5210000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5260000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5290000</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5300000</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5360000</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5370000</v>
+      </c>
+      <c r="K3" s="2">
+        <v>5400000</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5400000</v>
+      </c>
+      <c r="M3" s="2">
+        <v>5410000</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5410000</v>
+      </c>
+      <c r="O3" s="2">
+        <v>5450000</v>
+      </c>
+      <c r="P3" s="2">
+        <v>5500000</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>5560000</v>
+      </c>
+      <c r="R3" s="2">
+        <v>5610000</v>
+      </c>
+      <c r="S3" s="2">
+        <v>5660000</v>
+      </c>
+      <c r="T3" s="2">
+        <v>5660000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3300000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3340000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3340000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3390000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3540000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3590000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3630000</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3640000</v>
+      </c>
+      <c r="L4" s="2">
+        <v>3690000</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3720000</v>
+      </c>
+      <c r="N4" s="2">
+        <v>3730000</v>
+      </c>
+      <c r="O4" s="2">
+        <v>3740000</v>
+      </c>
+      <c r="P4" s="2">
+        <v>3790000</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3830000</v>
+      </c>
+      <c r="R4" s="2">
+        <v>3890000</v>
+      </c>
+      <c r="S4" s="2">
+        <v>3890000</v>
+      </c>
+      <c r="T4" s="2">
+        <v>3900000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>21600000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>21400000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>21400000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>21400000</v>
+      </c>
+      <c r="F5" s="2">
+        <v>21500000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>21400000</v>
+      </c>
+      <c r="H5" s="2">
+        <v>21400000</v>
+      </c>
+      <c r="I5" s="2">
+        <v>20600000</v>
+      </c>
+      <c r="J5" s="2">
+        <v>20600000</v>
+      </c>
+      <c r="K5" s="2">
+        <v>20600000</v>
+      </c>
+      <c r="L5" s="2">
+        <v>20600000</v>
+      </c>
+      <c r="M5" s="2">
+        <v>20600000</v>
+      </c>
+      <c r="N5" s="2">
+        <v>20700000</v>
+      </c>
+      <c r="O5" s="2">
+        <v>20600000</v>
+      </c>
+      <c r="P5" s="2">
+        <v>20700000</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>20600000</v>
+      </c>
+      <c r="R5" s="2">
+        <v>20100000</v>
+      </c>
+      <c r="S5" s="2">
+        <v>19700000</v>
+      </c>
+      <c r="T5" s="2">
+        <v>19600000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="I6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="J6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="K6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="L6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="M6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="N6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="O6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="P6" s="2">
+        <v>8760000</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>8070000</v>
+      </c>
+      <c r="R6" s="2">
+        <v>7850000</v>
+      </c>
+      <c r="S6" s="2">
+        <v>7820000</v>
+      </c>
+      <c r="T6" s="2">
+        <v>7670000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1570000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1600000</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1640000</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1660000</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1660000</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1620000</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1620000</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1600000</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1520000</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1520000</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1520000</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1520000</v>
+      </c>
+      <c r="S7" s="2">
+        <v>1560000</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1560000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3300000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3300000</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3300000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3020000</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2750000</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2460000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2460000</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2980000</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2980000</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2980000</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2980000</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="P8" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="R8" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="S8" s="2">
+        <v>2160000</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2160000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4630000</v>
+      </c>
+      <c r="K9" s="2">
+        <v>8610000</v>
+      </c>
+      <c r="L9" s="2">
+        <v>8610000</v>
+      </c>
+      <c r="M9" s="2">
+        <v>8610000</v>
+      </c>
+      <c r="N9" s="2">
+        <v>8610000</v>
+      </c>
+      <c r="O9" s="2">
+        <v>4650000</v>
+      </c>
+      <c r="P9" s="2">
+        <v>4650000</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>8610000</v>
+      </c>
+      <c r="R9" s="2">
+        <v>7570000</v>
+      </c>
+      <c r="S9" s="2">
+        <v>7570000</v>
+      </c>
+      <c r="T9" s="2">
+        <v>7570000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5830000</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5800000</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5700000</v>
+      </c>
+      <c r="L10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5690000</v>
+      </c>
+      <c r="N10" s="2">
+        <v>5800000</v>
+      </c>
+      <c r="O10" s="2">
+        <v>5800000</v>
+      </c>
+      <c r="P10" s="2">
+        <v>5700000</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>5750000</v>
+      </c>
+      <c r="R10" s="2">
+        <v>5610000</v>
+      </c>
+      <c r="S10" s="2">
+        <v>5610000</v>
+      </c>
+      <c r="T10" s="2">
+        <v>5610000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3540000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3530000</v>
+      </c>
+      <c r="I11" s="2">
+        <v>3530000</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="K11" s="2">
+        <v>3490000</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="M11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="N11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="O11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="P11" s="2">
+        <v>3440000</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>3340000</v>
+      </c>
+      <c r="R11" s="2">
+        <v>3250000</v>
+      </c>
+      <c r="S11" s="2">
+        <v>3150000</v>
+      </c>
+      <c r="T11" s="2">
+        <v>3320000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7410000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7380000</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7230000</v>
+      </c>
+      <c r="E12" s="2">
+        <v>7380000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>6890000</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6790000</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6780000</v>
+      </c>
+      <c r="I12" s="2">
+        <v>6570000</v>
+      </c>
+      <c r="J12" s="2">
+        <v>6470000</v>
+      </c>
+      <c r="K12" s="2">
+        <v>6590000</v>
+      </c>
+      <c r="L12" s="2">
+        <v>6390000</v>
+      </c>
+      <c r="M12" s="2">
+        <v>5950000</v>
+      </c>
+      <c r="N12" s="2">
+        <v>6000000</v>
+      </c>
+      <c r="O12" s="2">
+        <v>5950000</v>
+      </c>
+      <c r="P12" s="2">
+        <v>5900000</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>5710000</v>
+      </c>
+      <c r="R12" s="2">
+        <v>5560000</v>
+      </c>
+      <c r="S12" s="2">
+        <v>5700000</v>
+      </c>
+      <c r="T12" s="2">
+        <v>5650000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10700000</v>
+      </c>
+      <c r="C13" s="2">
+        <v>10700000</v>
+      </c>
+      <c r="D13" s="2">
+        <v>10700000</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10600000</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10300000</v>
+      </c>
+      <c r="G13" s="2">
+        <v>10300000</v>
+      </c>
+      <c r="H13" s="2">
+        <v>10200000</v>
+      </c>
+      <c r="I13" s="2">
+        <v>9960000</v>
+      </c>
+      <c r="J13" s="2">
+        <v>9640000</v>
+      </c>
+      <c r="K13" s="2">
+        <v>9530000</v>
+      </c>
+      <c r="L13" s="2">
+        <v>9390000</v>
+      </c>
+      <c r="M13" s="2">
+        <v>9350000</v>
+      </c>
+      <c r="N13" s="2">
+        <v>9220000</v>
+      </c>
+      <c r="O13" s="2">
+        <v>9050000</v>
+      </c>
+      <c r="P13" s="2">
+        <v>9100000</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>8360000</v>
+      </c>
+      <c r="R13" s="2">
+        <v>8020000</v>
+      </c>
+      <c r="S13" s="2">
+        <v>7870000</v>
+      </c>
+      <c r="T13" s="2">
+        <v>8210000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2940000</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2950000</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2970000</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3140000</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3210000</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3250000</v>
+      </c>
+      <c r="K14" s="2">
+        <v>3200000</v>
+      </c>
+      <c r="L14" s="2">
+        <v>3150000</v>
+      </c>
+      <c r="M14" s="2">
+        <v>3100000</v>
+      </c>
+      <c r="N14" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3070000</v>
+      </c>
+      <c r="P14" s="2">
+        <v>3050000</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>2940000</v>
+      </c>
+      <c r="R14" s="2">
+        <v>2900000</v>
+      </c>
+      <c r="S14" s="2">
+        <v>2900000</v>
+      </c>
+      <c r="T14" s="2">
+        <v>2870000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3890000</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3890000</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3910000</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3910000</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="I15" s="2">
+        <v>3930000</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3980000</v>
+      </c>
+      <c r="K15" s="2">
+        <v>4110000</v>
+      </c>
+      <c r="L15" s="2">
+        <v>4080000</v>
+      </c>
+      <c r="M15" s="2">
+        <v>4080000</v>
+      </c>
+      <c r="N15" s="2">
+        <v>4130000</v>
+      </c>
+      <c r="O15" s="2">
+        <v>4110000</v>
+      </c>
+      <c r="P15" s="2">
+        <v>4180000</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>4180000</v>
+      </c>
+      <c r="R15" s="2">
+        <v>4130000</v>
+      </c>
+      <c r="S15" s="2">
+        <v>4160000</v>
+      </c>
+      <c r="T15" s="2">
+        <v>4160000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1630000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1650000</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1650000</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1670000</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1670000</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1700000</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1780000</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1870000</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1870000</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1850000</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1940000</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1940000</v>
+      </c>
+      <c r="N16" s="2">
+        <v>2010000</v>
+      </c>
+      <c r="O16" s="2">
+        <v>2030000</v>
+      </c>
+      <c r="P16" s="2">
+        <v>2030000</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>2030000</v>
+      </c>
+      <c r="R16" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="S16" s="2">
+        <v>2040000</v>
+      </c>
+      <c r="T16" s="2">
+        <v>2040000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2710000</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="G17" s="2">
+        <v>280000</v>
+      </c>
+      <c r="H17" s="2">
+        <v>280000</v>
+      </c>
+      <c r="I17" s="2">
+        <v>280000</v>
+      </c>
+      <c r="J17" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="L17" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="M17" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="N17" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="O17" s="2">
+        <v>2770000</v>
+      </c>
+      <c r="P17" s="2">
+        <v>2770000</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>280000</v>
+      </c>
+      <c r="R17" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="S17" s="2">
+        <v>2800000</v>
+      </c>
+      <c r="T17" s="2">
+        <v>2990000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4030000</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4030000</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4030000</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4110000</v>
+      </c>
+      <c r="F18" s="2">
+        <v>4180000</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4230000</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4380000</v>
+      </c>
+      <c r="I18" s="2">
+        <v>4430000</v>
+      </c>
+      <c r="J18" s="2">
+        <v>4500000</v>
+      </c>
+      <c r="K18" s="2">
+        <v>4480000</v>
+      </c>
+      <c r="L18" s="2">
+        <v>4470000</v>
+      </c>
+      <c r="M18" s="2">
+        <v>4520000</v>
+      </c>
+      <c r="N18" s="2">
+        <v>4530000</v>
+      </c>
+      <c r="O18" s="2">
+        <v>4550000</v>
+      </c>
+      <c r="P18" s="2">
+        <v>4600000</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>4530000</v>
+      </c>
+      <c r="R18" s="2">
+        <v>4590000</v>
+      </c>
+      <c r="S18" s="2">
+        <v>4620000</v>
+      </c>
+      <c r="T18" s="2">
+        <v>4670000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chavez Lopez First Commit
</commit_message>
<xml_diff>
--- a/Datos_colonia.xlsx
+++ b/Datos_colonia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\IA\ia_dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\ia_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF373784-40B0-45F0-B320-6B99E9C812EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{978F42C7-E5DF-4C18-97CD-3E6B9CF32AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Loma bonita sur</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>independencia</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -161,9 +164,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +175,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -198,17 +209,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,16 +503,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
       <c r="B1" s="1">
         <v>44075</v>
       </c>
@@ -1799,7 +1814,7 @@
         <v>2750000</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1824,7 +1839,7 @@
       <c r="H22" s="2">
         <v>3200000</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="5">
         <v>3210000</v>
       </c>
       <c r="J22" s="2">
@@ -3317,5 +3332,6 @@
     <sortCondition ref="B2:B44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>